<commit_message>
Atualização de arquivos de outro computador
</commit_message>
<xml_diff>
--- a/Modelagem de Dados/Ubuntu School/Tabela de Dados a serem coletados (Ubuntu).xlsx
+++ b/Modelagem de Dados/Ubuntu School/Tabela de Dados a serem coletados (Ubuntu).xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="11_92D097E7ADB8A1151D8BD037355C485F0AEB40FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9954BFA1-B061-4BA1-BC25-711DC1FDC170}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" calcMode="manual"/>
+  <calcPr calcId="125725" calcMode="manual" calcCompleted="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="163">
   <si>
     <t>Atributo</t>
   </si>
@@ -489,16 +490,31 @@
   </si>
   <si>
     <t>senha_aluno</t>
+  </si>
+  <si>
+    <t>professor_aplicativo</t>
+  </si>
+  <si>
+    <t>sobrenome_prof</t>
+  </si>
+  <si>
+    <t>nome_prof</t>
+  </si>
+  <si>
+    <t>email_prof</t>
+  </si>
+  <si>
+    <t>senha_prof</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="##&quot;/&quot;##&quot;/&quot;####"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -728,7 +744,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -891,6 +907,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -907,28 +932,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Incorreto" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Ruim" xfId="1" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -966,9 +993,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1000,9 +1027,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1034,9 +1079,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1209,14 +1272,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
@@ -1229,40 +1292,42 @@
     <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.7109375" customWidth="1"/>
-    <col min="16" max="16" width="15" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:20">
-      <c r="A4" s="67" t="s">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="70" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="H4" s="67" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="H4" s="70" t="s">
         <v>154</v>
       </c>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
       <c r="N4" s="25"/>
-      <c r="O4" s="67" t="s">
+      <c r="O4" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="P4" s="70"/>
+      <c r="Q4" s="70"/>
+      <c r="R4" s="70"/>
+      <c r="S4" s="70"/>
+      <c r="T4" s="70"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1319,7 +1384,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1364,7 +1429,7 @@
       </c>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -1389,7 +1454,7 @@
       <c r="K7" s="12">
         <v>15</v>
       </c>
-      <c r="L7" s="71" t="s">
+      <c r="L7" s="66" t="s">
         <v>25</v>
       </c>
       <c r="M7" s="12"/>
@@ -1409,7 +1474,7 @@
       </c>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -1434,7 +1499,7 @@
       <c r="K8" s="2">
         <v>20</v>
       </c>
-      <c r="L8" s="71" t="s">
+      <c r="L8" s="66" t="s">
         <v>25</v>
       </c>
       <c r="M8" s="2"/>
@@ -1454,7 +1519,7 @@
       </c>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -1479,11 +1544,11 @@
       <c r="K9" s="2">
         <v>50</v>
       </c>
-      <c r="L9" s="71" t="s">
+      <c r="L9" s="66" t="s">
         <v>25</v>
       </c>
       <c r="M9" s="2"/>
-      <c r="N9" s="70"/>
+      <c r="N9" s="65"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2" t="s">
         <v>21</v>
@@ -1499,7 +1564,7 @@
       </c>
       <c r="T9" s="11"/>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
@@ -1522,14 +1587,14 @@
         <v>23</v>
       </c>
       <c r="K10" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>25</v>
       </c>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
         <v>12</v>
@@ -1544,16 +1609,16 @@
         <v>25</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="O11" s="67" t="s">
+      <c r="O11" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="P11" s="67"/>
-      <c r="Q11" s="67"/>
-      <c r="R11" s="67"/>
-      <c r="S11" s="67"/>
-      <c r="T11" s="67"/>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="P11" s="70"/>
+      <c r="Q11" s="70"/>
+      <c r="R11" s="70"/>
+      <c r="S11" s="70"/>
+      <c r="T11" s="70"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>13</v>
@@ -1566,6 +1631,14 @@
         <v>25</v>
       </c>
       <c r="F12" s="2"/>
+      <c r="H12" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="I12" s="70"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="70"/>
+      <c r="M12" s="70"/>
       <c r="O12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1585,7 +1658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>14</v>
@@ -1600,6 +1673,24 @@
         <v>25</v>
       </c>
       <c r="F13" s="2"/>
+      <c r="H13" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="64" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="M13" s="64" t="s">
+        <v>5</v>
+      </c>
       <c r="O13" s="12" t="s">
         <v>10</v>
       </c>
@@ -1615,7 +1706,7 @@
       </c>
       <c r="T13" s="12"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
         <v>15</v>
@@ -1630,6 +1721,20 @@
         <v>25</v>
       </c>
       <c r="F14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2" t="s">
         <v>143</v>
@@ -1645,7 +1750,7 @@
       </c>
       <c r="T14" s="2"/>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
         <v>16</v>
@@ -1660,6 +1765,20 @@
         <v>26</v>
       </c>
       <c r="F15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="2">
+        <v>20</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2" t="s">
         <v>144</v>
@@ -1673,7 +1792,7 @@
       </c>
       <c r="T15" s="2"/>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
         <v>31</v>
@@ -1688,6 +1807,20 @@
         <v>26</v>
       </c>
       <c r="F16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="2">
+        <v>20</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="2"/>
       <c r="O16" s="2" t="s">
         <v>18</v>
       </c>
@@ -1703,7 +1836,7 @@
       </c>
       <c r="T16" s="2"/>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="12" t="s">
         <v>140</v>
@@ -1718,6 +1851,20 @@
       <c r="F17" s="58" t="s">
         <v>141</v>
       </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="2">
+        <v>60</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="2"/>
       <c r="O17" s="2" t="s">
         <v>18</v>
       </c>
@@ -1733,7 +1880,7 @@
       </c>
       <c r="T17" s="2"/>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="61"/>
       <c r="B18" s="60"/>
       <c r="C18" s="60"/>
@@ -1742,14 +1889,22 @@
       <c r="F18" s="62" t="s">
         <v>142</v>
       </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="7"/>
-    </row>
-    <row r="19" spans="1:20">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="2">
+        <v>15</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>18</v>
       </c>
@@ -1771,7 +1926,7 @@
       <c r="L19" s="30"/>
       <c r="M19" s="7"/>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1793,7 +1948,7 @@
       <c r="L20" s="30"/>
       <c r="M20" s="7"/>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -1815,26 +1970,26 @@
       <c r="L21" s="30"/>
       <c r="M21" s="8"/>
     </row>
-    <row r="22" spans="1:20" s="68" customFormat="1"/>
-    <row r="23" spans="1:20">
-      <c r="A23" s="67" t="s">
+    <row r="22" spans="1:20" s="71" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="70" t="s">
         <v>138</v>
       </c>
-      <c r="B23" s="67"/>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-      <c r="H23" s="67" t="s">
+      <c r="B23" s="70"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="70"/>
+      <c r="F23" s="70"/>
+      <c r="H23" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
-      <c r="K23" s="67"/>
-      <c r="L23" s="67"/>
-      <c r="M23" s="67"/>
-    </row>
-    <row r="24" spans="1:20">
+      <c r="I23" s="70"/>
+      <c r="J23" s="70"/>
+      <c r="K23" s="70"/>
+      <c r="L23" s="70"/>
+      <c r="M23" s="70"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
@@ -1872,12 +2027,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>22</v>
@@ -1902,7 +2057,7 @@
       </c>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
         <v>29</v>
@@ -1932,7 +2087,7 @@
       </c>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
         <v>33</v>
@@ -1947,8 +2102,14 @@
         <v>25</v>
       </c>
       <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:20">
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
         <v>34</v>
@@ -1964,7 +2125,7 @@
       </c>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
         <v>35</v>
@@ -1978,7 +2139,7 @@
       </c>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
         <v>36</v>
@@ -1993,16 +2154,16 @@
         <v>25</v>
       </c>
       <c r="F30" s="2"/>
-      <c r="H30" s="64" t="s">
+      <c r="H30" s="67" t="s">
         <v>153</v>
       </c>
-      <c r="I30" s="65"/>
-      <c r="J30" s="65"/>
-      <c r="K30" s="65"/>
-      <c r="L30" s="65"/>
-      <c r="M30" s="66"/>
-    </row>
-    <row r="31" spans="1:20">
+      <c r="I30" s="68"/>
+      <c r="J30" s="68"/>
+      <c r="K30" s="68"/>
+      <c r="L30" s="68"/>
+      <c r="M30" s="69"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
         <v>37</v>
@@ -2036,7 +2197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
         <v>30</v>
@@ -2066,7 +2227,7 @@
       </c>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
         <v>32</v>
@@ -2096,7 +2257,7 @@
       </c>
       <c r="M33" s="2"/>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="12" t="s">
         <v>152</v>
@@ -2126,7 +2287,7 @@
       </c>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:20" s="63" customFormat="1">
+    <row r="35" spans="1:20" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="61"/>
       <c r="B35" s="60"/>
       <c r="C35" s="60"/>
@@ -2142,12 +2303,12 @@
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>22</v>
@@ -2158,7 +2319,7 @@
       </c>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="63"/>
       <c r="B37" s="63"/>
       <c r="C37" s="63"/>
@@ -2166,17 +2327,17 @@
       <c r="E37" s="63"/>
       <c r="F37" s="63"/>
     </row>
-    <row r="38" spans="1:20">
-      <c r="H38" s="67" t="s">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="H38" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="I38" s="67"/>
-      <c r="J38" s="67"/>
-      <c r="K38" s="67"/>
-      <c r="L38" s="67"/>
-      <c r="M38" s="67"/>
-    </row>
-    <row r="39" spans="1:20">
+      <c r="I38" s="70"/>
+      <c r="J38" s="70"/>
+      <c r="K38" s="70"/>
+      <c r="L38" s="70"/>
+      <c r="M38" s="70"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H39" s="1" t="s">
         <v>1</v>
       </c>
@@ -2196,7 +2357,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H40" s="2" t="s">
         <v>10</v>
       </c>
@@ -2212,7 +2373,7 @@
       </c>
       <c r="M40" s="2"/>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H41" s="2" t="s">
         <v>18</v>
       </c>
@@ -2228,15 +2389,15 @@
       </c>
       <c r="M41" s="2"/>
     </row>
-    <row r="42" spans="1:20">
-      <c r="A42" s="64" t="s">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="67" t="s">
         <v>145</v>
       </c>
-      <c r="B42" s="65"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="66"/>
+      <c r="B42" s="68"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="68"/>
+      <c r="F42" s="69"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2" t="s">
         <v>77</v>
@@ -2250,7 +2411,7 @@
       </c>
       <c r="M42" s="2"/>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="54" t="s">
         <v>1</v>
       </c>
@@ -2282,7 +2443,7 @@
       </c>
       <c r="M43" s="2"/>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>10</v>
       </c>
@@ -2312,7 +2473,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
         <v>147</v>
@@ -2342,7 +2503,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
         <v>148</v>
@@ -2370,7 +2531,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
         <v>149</v>
@@ -2393,7 +2554,7 @@
       </c>
       <c r="T47" s="56"/>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
         <v>150</v>
@@ -2423,7 +2584,7 @@
       </c>
       <c r="M48" s="2"/>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
         <v>151</v>
@@ -2445,7 +2606,7 @@
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
     </row>
-    <row r="50" spans="1:13" s="55" customFormat="1">
+    <row r="50" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50"/>
@@ -2459,7 +2620,7 @@
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="55"/>
       <c r="B52" s="55"/>
       <c r="C52" s="55"/>
@@ -2467,9 +2628,9 @@
       <c r="E52" s="55"/>
       <c r="F52" s="55"/>
     </row>
-    <row r="56" spans="1:13" ht="15" customHeight="1"/>
+    <row r="56" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="A42:F42"/>
     <mergeCell ref="H38:M38"/>
     <mergeCell ref="O4:T4"/>
@@ -2480,6 +2641,7 @@
     <mergeCell ref="H23:M23"/>
     <mergeCell ref="H30:M30"/>
     <mergeCell ref="H4:M4"/>
+    <mergeCell ref="H12:M12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId1"/>
@@ -2487,14 +2649,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:T67"/>
   <sheetViews>
     <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
@@ -2517,31 +2679,31 @@
     <col min="20" max="20" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20">
-      <c r="B2" s="69" t="s">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" s="72" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="Q2" s="64" t="s">
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
+      <c r="Q2" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="66"/>
-    </row>
-    <row r="3" spans="2:20">
+      <c r="R2" s="68"/>
+      <c r="S2" s="68"/>
+      <c r="T2" s="69"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
         <v>6</v>
       </c>
@@ -2597,7 +2759,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:20">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="18">
         <v>54206</v>
       </c>
@@ -2654,7 +2816,7 @@
         <v>11965654852</v>
       </c>
     </row>
-    <row r="5" spans="2:20">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="18">
         <f>B4+1</f>
         <v>54207</v>
@@ -2714,7 +2876,7 @@
         <v>11987564321</v>
       </c>
     </row>
-    <row r="6" spans="2:20">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="18">
         <f t="shared" ref="B6:B8" si="0">B5+1</f>
         <v>54208</v>
@@ -2774,7 +2936,7 @@
         <v>11965874236</v>
       </c>
     </row>
-    <row r="7" spans="2:20">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="18">
         <f t="shared" si="0"/>
         <v>54209</v>
@@ -2834,7 +2996,7 @@
         <v>11955498421</v>
       </c>
     </row>
-    <row r="8" spans="2:20">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="18">
         <f t="shared" si="0"/>
         <v>54210</v>
@@ -2894,7 +3056,7 @@
         <v>11923456122</v>
       </c>
     </row>
-    <row r="9" spans="2:20">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
         <v>10</v>
       </c>
@@ -2921,7 +3083,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:20">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -2930,7 +3092,7 @@
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
     </row>
-    <row r="11" spans="2:20">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -2939,7 +3101,7 @@
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="2:20">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -2948,22 +3110,22 @@
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
     </row>
-    <row r="13" spans="2:20">
-      <c r="B13" s="67" t="s">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="G13" s="64" t="s">
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="G13" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="66"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="69"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
     </row>
-    <row r="14" spans="2:20">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="24" t="s">
         <v>69</v>
       </c>
@@ -2988,7 +3150,7 @@
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
     </row>
-    <row r="15" spans="2:20">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" s="18">
         <v>100</v>
       </c>
@@ -3013,7 +3175,7 @@
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
     </row>
-    <row r="16" spans="2:20">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="18">
         <v>101</v>
       </c>
@@ -3038,7 +3200,7 @@
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
     </row>
-    <row r="17" spans="2:14">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="18">
         <v>102</v>
       </c>
@@ -3063,7 +3225,7 @@
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
     </row>
-    <row r="18" spans="2:14">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="22" t="s">
         <v>10</v>
       </c>
@@ -3086,7 +3248,7 @@
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
     </row>
-    <row r="19" spans="2:14">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G19" s="22" t="s">
         <v>10</v>
       </c>
@@ -3100,7 +3262,7 @@
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
     </row>
-    <row r="20" spans="2:14">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
@@ -3109,7 +3271,7 @@
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
     </row>
-    <row r="21" spans="2:14">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -3118,25 +3280,25 @@
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
     </row>
-    <row r="24" spans="2:14">
-      <c r="B24" s="67" t="s">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="70" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="67"/>
-      <c r="M24" s="64" t="s">
+      <c r="C24" s="70"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="70"/>
+      <c r="J24" s="70"/>
+      <c r="K24" s="70"/>
+      <c r="M24" s="67" t="s">
         <v>103</v>
       </c>
-      <c r="N24" s="65"/>
-    </row>
-    <row r="25" spans="2:14">
+      <c r="N24" s="68"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
         <v>28</v>
       </c>
@@ -3174,7 +3336,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="2:14">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="18">
         <v>5001</v>
       </c>
@@ -3212,7 +3374,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="2:14">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="18">
         <f>B26+1</f>
         <v>5002</v>
@@ -3251,7 +3413,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="2:14">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="18">
         <f t="shared" ref="B28:B29" si="2">B27+1</f>
         <v>5003</v>
@@ -3290,7 +3452,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="2:14">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="18">
         <f t="shared" si="2"/>
         <v>5004</v>
@@ -3326,7 +3488,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="2:14">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="22" t="s">
         <v>10</v>
       </c>
@@ -3338,36 +3500,36 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="2:14">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="43"/>
       <c r="E31" s="44"/>
     </row>
-    <row r="32" spans="2:14">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E32" s="44"/>
     </row>
-    <row r="33" spans="2:18">
-      <c r="B33" s="67" t="s">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B33" s="70" t="s">
         <v>114</v>
       </c>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="67"/>
-      <c r="G33" s="67" t="s">
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
+      <c r="G33" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="H33" s="67"/>
-      <c r="I33" s="67"/>
-      <c r="J33" s="67"/>
-      <c r="K33" s="67"/>
-      <c r="L33" s="67"/>
-      <c r="M33" s="67"/>
-      <c r="N33" s="67"/>
-      <c r="O33" s="67"/>
-      <c r="P33" s="67"/>
-      <c r="Q33" s="67"/>
-      <c r="R33" s="67"/>
-    </row>
-    <row r="34" spans="2:18">
+      <c r="H33" s="70"/>
+      <c r="I33" s="70"/>
+      <c r="J33" s="70"/>
+      <c r="K33" s="70"/>
+      <c r="L33" s="70"/>
+      <c r="M33" s="70"/>
+      <c r="N33" s="70"/>
+      <c r="O33" s="70"/>
+      <c r="P33" s="70"/>
+      <c r="Q33" s="70"/>
+      <c r="R33" s="70"/>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="26" t="s">
         <v>53</v>
       </c>
@@ -3417,7 +3579,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="2:18">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="18">
         <v>500</v>
       </c>
@@ -3465,7 +3627,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="2:18">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="18">
         <v>501</v>
       </c>
@@ -3511,7 +3673,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="2:18">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="18">
         <v>502</v>
       </c>
@@ -3528,7 +3690,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="2:18">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B38" s="18">
         <v>503</v>
       </c>
@@ -3545,7 +3707,7 @@
       <c r="P38" s="44"/>
       <c r="Q38" s="44"/>
     </row>
-    <row r="39" spans="2:18">
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B39" s="22" t="s">
         <v>10</v>
       </c>
@@ -3553,25 +3715,25 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="2:14">
-      <c r="B50" s="64" t="s">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B50" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="C50" s="65"/>
-      <c r="D50" s="65"/>
-      <c r="E50" s="65"/>
-      <c r="F50" s="65"/>
-      <c r="G50" s="66"/>
-      <c r="I50" s="64" t="s">
+      <c r="C50" s="68"/>
+      <c r="D50" s="68"/>
+      <c r="E50" s="68"/>
+      <c r="F50" s="68"/>
+      <c r="G50" s="69"/>
+      <c r="I50" s="67" t="s">
         <v>130</v>
       </c>
-      <c r="J50" s="65"/>
-      <c r="K50" s="65"/>
-      <c r="L50" s="65"/>
-      <c r="M50" s="65"/>
-      <c r="N50" s="66"/>
-    </row>
-    <row r="51" spans="2:14">
+      <c r="J50" s="68"/>
+      <c r="K50" s="68"/>
+      <c r="L50" s="68"/>
+      <c r="M50" s="68"/>
+      <c r="N50" s="69"/>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B51" s="26" t="s">
         <v>17</v>
       </c>
@@ -3609,7 +3771,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="2:14">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B52" s="18">
         <v>1</v>
       </c>
@@ -3647,7 +3809,7 @@
         <v>20001</v>
       </c>
     </row>
-    <row r="53" spans="2:14">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B53" s="18">
         <v>2</v>
       </c>
@@ -3685,7 +3847,7 @@
         <v>20002</v>
       </c>
     </row>
-    <row r="54" spans="2:14">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B54" s="48">
         <v>3</v>
       </c>
@@ -3711,7 +3873,7 @@
       <c r="M54" s="27"/>
       <c r="N54" s="49"/>
     </row>
-    <row r="55" spans="2:14">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B55" s="50" t="s">
         <v>10</v>
       </c>
@@ -3726,28 +3888,28 @@
       </c>
       <c r="H55" s="8"/>
     </row>
-    <row r="56" spans="2:14">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B56" s="27"/>
     </row>
-    <row r="58" spans="2:14">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B58" s="7"/>
     </row>
-    <row r="59" spans="2:14">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B59" s="7"/>
     </row>
-    <row r="60" spans="2:14">
-      <c r="B60" s="67" t="s">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B60" s="70" t="s">
         <v>137</v>
       </c>
-      <c r="C60" s="67"/>
-      <c r="D60" s="67"/>
-      <c r="E60" s="67"/>
-      <c r="F60" s="67"/>
-      <c r="G60" s="67"/>
-      <c r="H60" s="67"/>
-      <c r="I60" s="67"/>
-    </row>
-    <row r="61" spans="2:14">
+      <c r="C60" s="70"/>
+      <c r="D60" s="70"/>
+      <c r="E60" s="70"/>
+      <c r="F60" s="70"/>
+      <c r="G60" s="70"/>
+      <c r="H60" s="70"/>
+      <c r="I60" s="70"/>
+    </row>
+    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B61" s="26" t="s">
         <v>76</v>
       </c>
@@ -3773,7 +3935,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="2:14">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B62" s="18">
         <v>1000</v>
       </c>
@@ -3800,7 +3962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:14">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B63" s="18">
         <v>1000</v>
       </c>
@@ -3827,7 +3989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:14">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B64" s="18">
         <v>1000</v>
       </c>
@@ -3854,7 +4016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:9">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="18">
         <v>1001</v>
       </c>
@@ -3881,7 +4043,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="2:9">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="18">
         <v>1001</v>
       </c>
@@ -3908,7 +4070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:9">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="50" t="s">
         <v>10</v>
       </c>
@@ -3921,17 +4083,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="G33:R33"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="I50:N50"/>
+    <mergeCell ref="B60:I60"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="Q2:T2"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="G13:J13"/>
     <mergeCell ref="B24:K24"/>
     <mergeCell ref="M24:N24"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="G33:R33"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="I50:N50"/>
-    <mergeCell ref="B60:I60"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Commits atrasados - Novos JS e Novos Estudos (HTML, CSS e JS)
</commit_message>
<xml_diff>
--- a/Modelagem de Dados/Ubuntu School/Tabela de Dados a serem coletados (Ubuntu).xlsx
+++ b/Modelagem de Dados/Ubuntu School/Tabela de Dados a serem coletados (Ubuntu).xlsx
@@ -7,15 +7,15 @@
     <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="4" r:id="rId2"/>
+    <sheet name="Dados" sheetId="1" r:id="rId1"/>
+    <sheet name="Informações" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" calcMode="manual"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="163">
   <si>
     <t>Atributo</t>
   </si>
@@ -449,9 +449,6 @@
     <t>nome_turma</t>
   </si>
   <si>
-    <t>ano_turma</t>
-  </si>
-  <si>
     <t>Escola</t>
   </si>
   <si>
@@ -476,9 +473,6 @@
     <t>situacao_professor</t>
   </si>
   <si>
-    <t>Aula (ministradas)</t>
-  </si>
-  <si>
     <t>aluno_aplicativo</t>
   </si>
   <si>
@@ -489,6 +483,27 @@
   </si>
   <si>
     <t>senha_aluno</t>
+  </si>
+  <si>
+    <t>professor_aplicativo</t>
+  </si>
+  <si>
+    <t>id_professor</t>
+  </si>
+  <si>
+    <t>nome_prof</t>
+  </si>
+  <si>
+    <t>sobrenome_prof</t>
+  </si>
+  <si>
+    <t>email_prof</t>
+  </si>
+  <si>
+    <t>senha_prof</t>
+  </si>
+  <si>
+    <t>curso_turma</t>
   </si>
 </sst>
 </file>
@@ -728,7 +743,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -891,6 +906,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -903,16 +930,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1212,14 +1230,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:T56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" customWidth="1"/>
@@ -1229,38 +1247,38 @@
     <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.7109375" customWidth="1"/>
-    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:20">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="71" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="H4" s="67" t="s">
-        <v>154</v>
-      </c>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="H4" s="71" t="s">
+        <v>152</v>
+      </c>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="71"/>
+      <c r="M4" s="71"/>
       <c r="N4" s="25"/>
-      <c r="O4" s="67" t="s">
+      <c r="O4" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
+      <c r="P4" s="71"/>
+      <c r="Q4" s="71"/>
+      <c r="R4" s="71"/>
+      <c r="S4" s="71"/>
+      <c r="T4" s="71"/>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="1" t="s">
@@ -1389,7 +1407,7 @@
       <c r="K7" s="12">
         <v>15</v>
       </c>
-      <c r="L7" s="71" t="s">
+      <c r="L7" s="67" t="s">
         <v>25</v>
       </c>
       <c r="M7" s="12"/>
@@ -1426,7 +1444,7 @@
       <c r="F8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>23</v>
@@ -1434,7 +1452,7 @@
       <c r="K8" s="2">
         <v>20</v>
       </c>
-      <c r="L8" s="71" t="s">
+      <c r="L8" s="67" t="s">
         <v>25</v>
       </c>
       <c r="M8" s="2"/>
@@ -1471,7 +1489,7 @@
       <c r="F9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>23</v>
@@ -1479,11 +1497,11 @@
       <c r="K9" s="2">
         <v>50</v>
       </c>
-      <c r="L9" s="71" t="s">
+      <c r="L9" s="67" t="s">
         <v>25</v>
       </c>
       <c r="M9" s="2"/>
-      <c r="N9" s="70"/>
+      <c r="N9" s="66"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2" t="s">
         <v>21</v>
@@ -1516,7 +1534,7 @@
       <c r="F10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>23</v>
@@ -1544,14 +1562,14 @@
         <v>25</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="O11" s="67" t="s">
+      <c r="O11" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="P11" s="67"/>
-      <c r="Q11" s="67"/>
-      <c r="R11" s="67"/>
-      <c r="S11" s="67"/>
-      <c r="T11" s="67"/>
+      <c r="P11" s="71"/>
+      <c r="Q11" s="71"/>
+      <c r="R11" s="71"/>
+      <c r="S11" s="71"/>
+      <c r="T11" s="71"/>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="2"/>
@@ -1566,6 +1584,14 @@
         <v>25</v>
       </c>
       <c r="F12" s="2"/>
+      <c r="H12" s="71" t="s">
+        <v>156</v>
+      </c>
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="71"/>
       <c r="O12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1600,6 +1626,24 @@
         <v>25</v>
       </c>
       <c r="F13" s="2"/>
+      <c r="H13" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="64" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="M13" s="64" t="s">
+        <v>5</v>
+      </c>
       <c r="O13" s="12" t="s">
         <v>10</v>
       </c>
@@ -1630,6 +1674,20 @@
         <v>25</v>
       </c>
       <c r="F14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2" t="s">
         <v>143</v>
@@ -1660,9 +1718,23 @@
         <v>26</v>
       </c>
       <c r="F15" s="2"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="12">
+        <v>15</v>
+      </c>
+      <c r="L15" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="12"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="Q15" s="2" t="s">
         <v>22</v>
@@ -1688,11 +1760,25 @@
         <v>26</v>
       </c>
       <c r="F16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="2">
+        <v>20</v>
+      </c>
+      <c r="L16" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="2"/>
       <c r="O16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q16" s="2" t="s">
         <v>22</v>
@@ -1703,7 +1789,7 @@
       </c>
       <c r="T16" s="2"/>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:13">
       <c r="A17" s="12"/>
       <c r="B17" s="12" t="s">
         <v>140</v>
@@ -1718,22 +1804,22 @@
       <c r="F17" s="58" t="s">
         <v>141</v>
       </c>
-      <c r="O17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T17" s="2"/>
-    </row>
-    <row r="18" spans="1:20">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="2">
+        <v>50</v>
+      </c>
+      <c r="L17" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="61"/>
       <c r="B18" s="60"/>
       <c r="C18" s="60"/>
@@ -1742,28 +1828,36 @@
       <c r="F18" s="62" t="s">
         <v>142</v>
       </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="7"/>
-    </row>
-    <row r="19" spans="1:20">
-      <c r="A19" s="13" t="s">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="2">
+        <v>12</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="13" t="s">
+      <c r="B19" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="59" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="13"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="2"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
@@ -1771,21 +1865,21 @@
       <c r="L19" s="30"/>
       <c r="M19" s="7"/>
     </row>
-    <row r="20" spans="1:20">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:13">
+      <c r="A20" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="B20" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="2"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="13"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
@@ -1793,12 +1887,12 @@
       <c r="L20" s="30"/>
       <c r="M20" s="7"/>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:13">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>22</v>
@@ -1815,127 +1909,120 @@
       <c r="L21" s="30"/>
       <c r="M21" s="8"/>
     </row>
-    <row r="22" spans="1:20" s="68" customFormat="1"/>
-    <row r="23" spans="1:20">
-      <c r="A23" s="67" t="s">
+    <row r="22" spans="1:13" s="65" customFormat="1">
+      <c r="A22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="65"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="71" t="s">
         <v>138</v>
       </c>
-      <c r="B23" s="67"/>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-      <c r="H23" s="67" t="s">
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="H24" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
-      <c r="K23" s="67"/>
-      <c r="L23" s="67"/>
-      <c r="M23" s="67"/>
-    </row>
-    <row r="24" spans="1:20">
-      <c r="A24" s="1" t="s">
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="71"/>
+      <c r="L24" s="71"/>
+      <c r="M24" s="71"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="M25" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
-      <c r="A25" s="2" t="s">
+    <row r="26" spans="1:13">
+      <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" s="2"/>
-      <c r="H25" s="2" t="s">
+      <c r="D26" s="2"/>
+      <c r="E26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="H26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M25" s="2"/>
-    </row>
-    <row r="26" spans="1:20">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="2">
-        <v>50</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K26" s="2">
-        <v>50</v>
-      </c>
+      <c r="K26" s="2"/>
       <c r="L26" s="2" t="s">
         <v>25</v>
       </c>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:13">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>23</v>
@@ -1947,193 +2034,173 @@
         <v>25</v>
       </c>
       <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:20">
+      <c r="H27" s="2"/>
+      <c r="I27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" s="2">
+        <v>50</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="2">
-        <v>20</v>
-      </c>
-      <c r="E28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:20">
+      <c r="H28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="2">
+        <v>20</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="H29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:20">
+      <c r="K29" s="2"/>
+      <c r="L29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M29" s="2"/>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" s="2">
-        <v>2</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D30" s="2"/>
       <c r="E30" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F30" s="2"/>
-      <c r="H30" s="64" t="s">
-        <v>153</v>
-      </c>
-      <c r="I30" s="65"/>
-      <c r="J30" s="65"/>
-      <c r="K30" s="65"/>
-      <c r="L30" s="65"/>
-      <c r="M30" s="66"/>
-    </row>
-    <row r="31" spans="1:20">
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D31" s="2">
-        <v>10</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="F31" s="2"/>
-      <c r="H31" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="I31" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="J31" s="57" t="s">
-        <v>2</v>
-      </c>
-      <c r="K31" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="L31" s="57" t="s">
-        <v>4</v>
-      </c>
-      <c r="M31" s="57" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20">
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D32" s="2">
-        <v>15</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>25</v>
+        <v>10</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="F32" s="2"/>
-      <c r="H32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M32" s="2"/>
     </row>
     <row r="33" spans="1:20">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D33" s="2">
+        <v>15</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:20">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="2">
         <v>20</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" s="2"/>
-      <c r="H33" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J33" s="2" t="s">
+      <c r="E34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:20" s="63" customFormat="1">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C35" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M33" s="2"/>
-    </row>
-    <row r="34" spans="1:20">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F34" s="58" t="s">
+      <c r="D35" s="12"/>
+      <c r="E35" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="58" t="s">
         <v>141</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M34" s="2"/>
-    </row>
-    <row r="35" spans="1:20" s="63" customFormat="1">
-      <c r="A35" s="61"/>
-      <c r="B35" s="60"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="62" t="s">
-        <v>142</v>
       </c>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
@@ -2143,38 +2210,46 @@
       <c r="M35" s="7"/>
     </row>
     <row r="36" spans="1:20">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="61"/>
+      <c r="B36" s="60"/>
+      <c r="C36" s="60"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="62" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20">
+      <c r="A37" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="B37" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:20">
-      <c r="A37" s="63"/>
-      <c r="B37" s="63"/>
-      <c r="C37" s="63"/>
-      <c r="D37" s="63"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="2"/>
     </row>
     <row r="38" spans="1:20">
-      <c r="H38" s="67" t="s">
+      <c r="A38" s="63"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="63"/>
+      <c r="H38" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="I38" s="67"/>
-      <c r="J38" s="67"/>
-      <c r="K38" s="67"/>
-      <c r="L38" s="67"/>
-      <c r="M38" s="67"/>
+      <c r="I38" s="71"/>
+      <c r="J38" s="71"/>
+      <c r="K38" s="71"/>
+      <c r="L38" s="71"/>
+      <c r="M38" s="71"/>
     </row>
     <row r="39" spans="1:20">
       <c r="H39" s="1" t="s">
@@ -2229,14 +2304,6 @@
       <c r="M41" s="2"/>
     </row>
     <row r="42" spans="1:20">
-      <c r="A42" s="64" t="s">
-        <v>145</v>
-      </c>
-      <c r="B42" s="65"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="66"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2" t="s">
         <v>77</v>
@@ -2251,24 +2318,14 @@
       <c r="M42" s="2"/>
     </row>
     <row r="43" spans="1:20">
-      <c r="A43" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" s="54" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="E43" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F43" s="54" t="s">
-        <v>5</v>
-      </c>
+      <c r="A43" s="68" t="s">
+        <v>144</v>
+      </c>
+      <c r="B43" s="69"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="69"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="70"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2" t="s">
         <v>80</v>
@@ -2283,20 +2340,24 @@
       <c r="M43" s="2"/>
     </row>
     <row r="44" spans="1:20">
-      <c r="A44" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F44" s="2"/>
+      <c r="A44" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" s="54" t="s">
+        <v>5</v>
+      </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2" t="s">
         <v>81</v>
@@ -2313,16 +2374,16 @@
       </c>
     </row>
     <row r="45" spans="1:20">
-      <c r="A45" s="2"/>
+      <c r="A45" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B45" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D45" s="2">
-        <v>50</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D45" s="2"/>
       <c r="E45" s="5" t="s">
         <v>25</v>
       </c>
@@ -2345,15 +2406,15 @@
     <row r="46" spans="1:20">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D46" s="2">
-        <v>20</v>
-      </c>
-      <c r="E46" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F46" s="2"/>
@@ -2373,13 +2434,15 @@
     <row r="47" spans="1:20">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="2">
+        <v>20</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F47" s="2"/>
@@ -2396,14 +2459,12 @@
     <row r="48" spans="1:20">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D48" s="2">
-        <v>2</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D48" s="2"/>
       <c r="E48" s="5" t="s">
         <v>25</v>
       </c>
@@ -2412,7 +2473,7 @@
         <v>18</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>22</v>
@@ -2426,16 +2487,16 @@
     <row r="49" spans="1:13">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D49" s="2">
-        <v>10</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="F49" s="2"/>
       <c r="H49" s="2"/>
@@ -2446,12 +2507,20 @@
       <c r="M49" s="2"/>
     </row>
     <row r="50" spans="1:13" s="55" customFormat="1">
-      <c r="A50"/>
-      <c r="B50"/>
-      <c r="C50"/>
-      <c r="D50"/>
-      <c r="E50"/>
-      <c r="F50"/>
+      <c r="A50" s="2"/>
+      <c r="B50" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="2">
+        <v>10</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" s="2"/>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -2459,27 +2528,26 @@
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
     </row>
-    <row r="52" spans="1:13">
-      <c r="A52" s="55"/>
-      <c r="B52" s="55"/>
-      <c r="C52" s="55"/>
-      <c r="D52" s="55"/>
-      <c r="E52" s="55"/>
-      <c r="F52" s="55"/>
+    <row r="53" spans="1:13">
+      <c r="A53" s="55"/>
+      <c r="B53" s="55"/>
+      <c r="C53" s="55"/>
+      <c r="D53" s="55"/>
+      <c r="E53" s="55"/>
+      <c r="F53" s="55"/>
     </row>
     <row r="56" spans="1:13" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A42:F42"/>
+  <mergeCells count="9">
+    <mergeCell ref="A43:F43"/>
     <mergeCell ref="H38:M38"/>
     <mergeCell ref="O4:T4"/>
     <mergeCell ref="O11:T11"/>
-    <mergeCell ref="A22:XFD22"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="H24:M24"/>
     <mergeCell ref="H4:M4"/>
+    <mergeCell ref="H12:M12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId1"/>
@@ -2491,7 +2559,7 @@
   <dimension ref="B2:T67"/>
   <sheetViews>
     <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2518,28 +2586,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="72" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="Q2" s="64" t="s">
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
+      <c r="Q2" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="66"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="70"/>
     </row>
     <row r="3" spans="2:20">
       <c r="B3" s="17" t="s">
@@ -2949,17 +3017,17 @@
       <c r="L12" s="8"/>
     </row>
     <row r="13" spans="2:20">
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="G13" s="64" t="s">
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
+      <c r="G13" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="66"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="70"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
     </row>
@@ -3119,22 +3187,22 @@
       <c r="L21" s="8"/>
     </row>
     <row r="24" spans="2:14">
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="71" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="67"/>
-      <c r="M24" s="64" t="s">
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="71"/>
+      <c r="M24" s="68" t="s">
         <v>103</v>
       </c>
-      <c r="N24" s="65"/>
+      <c r="N24" s="69"/>
     </row>
     <row r="25" spans="2:14">
       <c r="B25" s="26" t="s">
@@ -3346,26 +3414,26 @@
       <c r="E32" s="44"/>
     </row>
     <row r="33" spans="2:18">
-      <c r="B33" s="67" t="s">
+      <c r="B33" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="67"/>
-      <c r="G33" s="67" t="s">
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="G33" s="71" t="s">
         <v>115</v>
       </c>
-      <c r="H33" s="67"/>
-      <c r="I33" s="67"/>
-      <c r="J33" s="67"/>
-      <c r="K33" s="67"/>
-      <c r="L33" s="67"/>
-      <c r="M33" s="67"/>
-      <c r="N33" s="67"/>
-      <c r="O33" s="67"/>
-      <c r="P33" s="67"/>
-      <c r="Q33" s="67"/>
-      <c r="R33" s="67"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="71"/>
+      <c r="J33" s="71"/>
+      <c r="K33" s="71"/>
+      <c r="L33" s="71"/>
+      <c r="M33" s="71"/>
+      <c r="N33" s="71"/>
+      <c r="O33" s="71"/>
+      <c r="P33" s="71"/>
+      <c r="Q33" s="71"/>
+      <c r="R33" s="71"/>
     </row>
     <row r="34" spans="2:18">
       <c r="B34" s="26" t="s">
@@ -3554,22 +3622,22 @@
       </c>
     </row>
     <row r="50" spans="2:14">
-      <c r="B50" s="64" t="s">
+      <c r="B50" s="68" t="s">
         <v>129</v>
       </c>
-      <c r="C50" s="65"/>
-      <c r="D50" s="65"/>
-      <c r="E50" s="65"/>
-      <c r="F50" s="65"/>
-      <c r="G50" s="66"/>
-      <c r="I50" s="64" t="s">
+      <c r="C50" s="69"/>
+      <c r="D50" s="69"/>
+      <c r="E50" s="69"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="70"/>
+      <c r="I50" s="68" t="s">
         <v>130</v>
       </c>
-      <c r="J50" s="65"/>
-      <c r="K50" s="65"/>
-      <c r="L50" s="65"/>
-      <c r="M50" s="65"/>
-      <c r="N50" s="66"/>
+      <c r="J50" s="69"/>
+      <c r="K50" s="69"/>
+      <c r="L50" s="69"/>
+      <c r="M50" s="69"/>
+      <c r="N50" s="70"/>
     </row>
     <row r="51" spans="2:14">
       <c r="B51" s="26" t="s">
@@ -3736,16 +3804,16 @@
       <c r="B59" s="7"/>
     </row>
     <row r="60" spans="2:14">
-      <c r="B60" s="67" t="s">
+      <c r="B60" s="71" t="s">
         <v>137</v>
       </c>
-      <c r="C60" s="67"/>
-      <c r="D60" s="67"/>
-      <c r="E60" s="67"/>
-      <c r="F60" s="67"/>
-      <c r="G60" s="67"/>
-      <c r="H60" s="67"/>
-      <c r="I60" s="67"/>
+      <c r="C60" s="71"/>
+      <c r="D60" s="71"/>
+      <c r="E60" s="71"/>
+      <c r="F60" s="71"/>
+      <c r="G60" s="71"/>
+      <c r="H60" s="71"/>
+      <c r="I60" s="71"/>
     </row>
     <row r="61" spans="2:14">
       <c r="B61" s="26" t="s">
@@ -3921,17 +3989,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="G33:R33"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="I50:N50"/>
+    <mergeCell ref="B60:I60"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="Q2:T2"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="G13:J13"/>
     <mergeCell ref="B24:K24"/>
     <mergeCell ref="M24:N24"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="G33:R33"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="I50:N50"/>
-    <mergeCell ref="B60:I60"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>